<commit_message>
refactor : relacing seeder name from sarpras to infrasctructure
</commit_message>
<xml_diff>
--- a/database/masters/base-seeder.xlsx
+++ b/database/masters/base-seeder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="module" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="46">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -60,10 +60,10 @@
     <t xml:space="preserve">describe</t>
   </si>
   <si>
-    <t xml:space="preserve">Sarpras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sarpras</t>
+    <t xml:space="preserve">Infrastructure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure</t>
   </si>
   <si>
     <t xml:space="preserve">account_balance_wallet</t>
@@ -102,22 +102,19 @@
     <t xml:space="preserve">Beranda</t>
   </si>
   <si>
-    <t xml:space="preserve">Sapras</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sarpras-dashboard</t>
+    <t xml:space="preserve">infrastructure-dashboard</t>
   </si>
   <si>
     <t xml:space="preserve">dashboard</t>
   </si>
   <si>
-    <t xml:space="preserve">Sarpras Unit</t>
+    <t xml:space="preserve">Infrastructure Unit</t>
   </si>
   <si>
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
-    <t xml:space="preserve">sarpras-unit</t>
+    <t xml:space="preserve">infrastructure-unit</t>
   </si>
   <si>
     <t xml:space="preserve">savings</t>
@@ -126,13 +123,13 @@
     <t xml:space="preserve">unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Sarpras Assets</t>
+    <t xml:space="preserve">Infrastructure Assets</t>
   </si>
   <si>
     <t xml:space="preserve">Assets</t>
   </si>
   <si>
-    <t xml:space="preserve">sarpras-assets</t>
+    <t xml:space="preserve">infrastructure-assets</t>
   </si>
   <si>
     <t xml:space="preserve">tune</t>
@@ -271,48 +268,52 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -506,91 +507,91 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B37:C37 A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="15.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="15.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="24.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="5" t="b">
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I2" s="5" t="b">
+      <c r="I2" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="J2" s="5" t="b">
+      <c r="J2" s="6" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -612,182 +613,182 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="1" sqref="B37:C37 E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="21.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="35.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="6" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="13.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="7" width="10.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.5"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="8" t="b">
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I2" s="8" t="b">
+      <c r="I2" s="9" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K2" s="8" t="b">
+      <c r="K2" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="8" t="b">
+      <c r="H3" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I3" s="8" t="b">
+      <c r="I3" s="9" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K3" s="8" t="b">
+      <c r="K3" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="H4" s="8" t="b">
+      <c r="H4" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="b">
+      <c r="I4" s="9" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="K4" s="8" t="b">
+      <c r="K4" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="K5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="K6" s="9"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="K6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E7" s="10"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="K7" s="9"/>
+      <c r="E7" s="11"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="K7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="K8" s="9"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="K8" s="10"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -807,67 +808,67 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="B37:C37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C37" activeCellId="0" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="50.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="50.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="10" t="s">
+    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="10"/>
+      <c r="B5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="10"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -889,36 +890,36 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="1" sqref="B37:C37 B38"/>
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -940,73 +941,73 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="1" sqref="B37:C37 C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>44</v>
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>44</v>
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>44</v>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1027,85 +1028,85 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="1" sqref="B37:C37 C5"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="39.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>46</v>
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>46</v>
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
feat : finnally adding asests and units-assets page
</commit_message>
<xml_diff>
--- a/database/masters/base-seeder.xlsx
+++ b/database/masters/base-seeder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="module" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -126,16 +126,28 @@
     <t xml:space="preserve">Infrastructure Unit Asset</t>
   </si>
   <si>
+    <t xml:space="preserve">Unit Asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infrastructure Asset</t>
+  </si>
+  <si>
     <t xml:space="preserve">Asset</t>
   </si>
   <si>
-    <t xml:space="preserve">infrastructure-unit-asset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tune</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unit/:unit/asset</t>
+    <t xml:space="preserve">infrastructure-asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset</t>
   </si>
   <si>
     <t xml:space="preserve">page</t>
@@ -627,8 +639,8 @@
   </sheetPr>
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J36" activeCellId="0" sqref="J36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -789,9 +801,39 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="K5" s="9"/>
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="H6" s="11"/>
@@ -827,8 +869,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -843,10 +885,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -857,7 +899,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -868,7 +910,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -879,10 +921,20 @@
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C7" s="12"/>
@@ -921,7 +973,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -929,7 +981,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -945,7 +997,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -953,7 +1005,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -975,7 +1027,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -990,10 +1042,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1004,7 +1056,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1015,7 +1067,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1026,12 +1078,19 @@
         <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="C5" s="5"/>
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>
@@ -1060,8 +1119,8 @@
   </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1077,13 +1136,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1094,10 +1153,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1108,10 +1167,10 @@
         <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1122,16 +1181,25 @@
         <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3"/>

</xml_diff>

<commit_message>
build : adding front end page for maintenance and document in each also for subunit pages
</commit_message>
<xml_diff>
--- a/database/masters/base-seeder.xlsx
+++ b/database/masters/base-seeder.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="69">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -138,6 +138,30 @@
     <t xml:space="preserve">unit/:unit/asset</t>
   </si>
   <si>
+    <t xml:space="preserve">Infrastructure Unit Asset Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset/:asset/document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infrastructure Unit Asset Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset/:asset/maintenance</t>
+  </si>
+  <si>
     <t xml:space="preserve">Infrastructure Asset</t>
   </si>
   <si>
@@ -150,6 +174,30 @@
     <t xml:space="preserve">asset</t>
   </si>
   <si>
+    <t xml:space="preserve">Infrastructure Asset Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset-document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset/:asset/document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infrastructure Asset Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset-maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset/:asset/maintenance</t>
+  </si>
+  <si>
     <t xml:space="preserve">page</t>
   </si>
   <si>
@@ -157,6 +205,9 @@
   </si>
   <si>
     <t xml:space="preserve">view</t>
+  </si>
+  <si>
+    <t xml:space="preserve">view, show</t>
   </si>
   <si>
     <t xml:space="preserve">view, create, show, update, delete, restore, destroy</t>
@@ -287,7 +338,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -329,10 +380,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -637,23 +684,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="24.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="7" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="26.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.5"/>
   </cols>
   <sheetData>
@@ -830,26 +877,162 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
+      <c r="J5" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="K5" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="K6" s="11"/>
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E7" s="12"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="K7" s="11"/>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I7" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="K8" s="11"/>
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I9" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -867,16 +1050,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="30.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="50.67"/>
   </cols>
   <sheetData>
@@ -885,10 +1068,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -898,8 +1081,8 @@
       <c r="B2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>43</v>
+      <c r="C2" s="11" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -910,7 +1093,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -921,7 +1104,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -932,14 +1115,53 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="12"/>
-    </row>
-    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -973,7 +1195,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -981,7 +1203,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -997,7 +1219,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1005,7 +1227,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1024,16 +1246,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="34.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.83"/>
   </cols>
   <sheetData>
@@ -1042,10 +1264,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1056,7 +1278,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1067,7 +1289,7 @@
         <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1078,7 +1300,7 @@
         <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1089,17 +1311,52 @@
         <v>39</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1117,16 +1374,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="19.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="39.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18"/>
   </cols>
@@ -1136,13 +1393,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1153,10 +1410,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1167,10 +1424,10 @@
         <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1181,10 +1438,10 @@
         <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1195,20 +1452,67 @@
         <v>39</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-    </row>
-    <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
+      <c r="C8" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
build : adding frontend page for maintenance tax and each own records for them
</commit_message>
<xml_diff>
--- a/database/masters/base-seeder.xlsx
+++ b/database/masters/base-seeder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="module" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="136">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -108,9 +108,6 @@
     <t xml:space="preserve">dashboard</t>
   </si>
   <si>
-    <t xml:space="preserve">Infrastructure Unit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unit</t>
   </si>
   <si>
@@ -123,7 +120,49 @@
     <t xml:space="preserve">unit</t>
   </si>
   <si>
-    <t xml:space="preserve">Infrastructure Unit Asset</t>
+    <t xml:space="preserve">Asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tune</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pajak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perawatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document</t>
   </si>
   <si>
     <t xml:space="preserve">Unit Asset</t>
@@ -132,15 +171,9 @@
     <t xml:space="preserve">infrastructure-unit-asset</t>
   </si>
   <si>
-    <t xml:space="preserve">tune</t>
-  </si>
-  <si>
     <t xml:space="preserve">unit/:unit/asset</t>
   </si>
   <si>
-    <t xml:space="preserve">Infrastructure Unit Asset Documents</t>
-  </si>
-  <si>
     <t xml:space="preserve">Unit Asset Documents</t>
   </si>
   <si>
@@ -150,64 +183,220 @@
     <t xml:space="preserve">unit/:unit/asset/:asset/document</t>
   </si>
   <si>
-    <t xml:space="preserve">Infrastructure Unit Asset Maintenance</t>
+    <t xml:space="preserve">Asset Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset-document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset/:asset/document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Perawatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset-maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset/:asset/maintenance</t>
   </si>
   <si>
     <t xml:space="preserve">Unit Asset Maintenance</t>
   </si>
   <si>
+    <t xml:space="preserve">Unit Asset Perawatan</t>
+  </si>
+  <si>
     <t xml:space="preserve">infrastructure-unit-asset-maintenance</t>
   </si>
   <si>
     <t xml:space="preserve">unit/:unit/asset/:asset/maintenance</t>
   </si>
   <si>
-    <t xml:space="preserve">Infrastructure Asset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infrastructure-asset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infrastructure Asset Documents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset Documents</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infrastructure-asset-document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asset/:asset/document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infrastructure Asset Maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asset Maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infrastructure-asset-maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">asset/:asset/maintenance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Infrastructure Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">infrastructure-document</t>
-  </si>
-  <si>
-    <t xml:space="preserve">document</t>
+    <t xml:space="preserve">Unit Asset Document Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Document Pajak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-document-maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset/:asset/document/:document/maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perawatan Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-document-maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document/:document/maintenance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Pajak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset-tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset/:asset/tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Pajak</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset/:asset/tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Document Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-document-tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset/:asset/document/:document/tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pajak Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-document-tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document/:document/tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tax Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pajak Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infrastructure-tax-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tax/:tax/record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Tax Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pajak Document Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-document-tax-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document/:document/tax/:tax/record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Tax Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Pajak Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-tax-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Document Tax Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Document Pajak Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-document-tax-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset/:asset/document/:document/tax/:tax/record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Tax Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Pajak Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset-tax-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset/:asset/tax/:tax/record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maintenance Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perawatan Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infrastructure-maintenance-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maintenance/:maintenance/record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Maintenance Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perawatan Document Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-document-maintenance-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">document/:document/maintenance/:maintenance/record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Maintenance Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Perawatan Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-maintenance-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Document Maintenance Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Asset Document Perawatan Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-asset-document-maintenance-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/asset/:asset/document/:document/maintenance/:maintenance/record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Maintenance Record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asset Perawatan Catatan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-asset-maintenance-record</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asset/:asset/maintenance/:maintenance/record</t>
   </si>
   <si>
     <t xml:space="preserve">page</t>
@@ -589,7 +778,7 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -696,23 +885,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="23.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="25.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="38.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="48.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="35.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="56.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="7" width="10.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="26.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="46.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="12.5"/>
   </cols>
   <sheetData>
@@ -773,12 +962,10 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="9" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I2" s="9" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H2" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9" t="b">
         <v>0</v>
       </c>
       <c r="K2" s="10" t="b">
@@ -794,27 +981,25 @@
         <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="9" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I3" s="9" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H3" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="I3" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="K3" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -826,33 +1011,28 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="9" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H4" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="9" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>29</v>
+      <c r="I4" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="K4" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -864,33 +1044,28 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="10" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I5" s="9" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H5" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>34</v>
+      <c r="I5" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="K5" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -902,33 +1077,28 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="10" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I6" s="9" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H6" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>34</v>
+      <c r="I6" s="9" t="b">
+        <v>1</v>
       </c>
       <c r="K6" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -940,29 +1110,27 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H7" s="10" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I7" s="9" t="n">
-        <f aca="false">FALSE()</f>
+      <c r="H7" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9" t="b">
         <v>0</v>
       </c>
       <c r="K7" s="10" t="b">
@@ -975,33 +1143,31 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H8" s="10" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I8" s="9" t="n">
-        <f aca="false">FALSE()</f>
+        <v>48</v>
+      </c>
+      <c r="H8" s="9" t="b">
         <v>0</v>
       </c>
+      <c r="I8" s="9" t="b">
+        <v>0</v>
+      </c>
       <c r="J8" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="K8" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1013,29 +1179,27 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="10" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I9" s="9" t="n">
-        <f aca="false">FALSE()</f>
+        <v>51</v>
+      </c>
+      <c r="H9" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9" t="b">
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
@@ -1051,35 +1215,834 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" s="10" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="I10" s="9" t="n">
-        <f aca="false">FALSE()</f>
+        <v>54</v>
+      </c>
+      <c r="H10" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9" t="b">
         <v>0</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="K10" s="10" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H12" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K13" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H14" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I15" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H16" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H17" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I17" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K18" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0"/>
+      <c r="B19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I19" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0"/>
+      <c r="B20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K20" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="L20" s="9"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0"/>
+      <c r="B21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H21" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K21" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0"/>
+      <c r="B22" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K22" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0"/>
+      <c r="B23" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K23" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="H24" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K24" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K25" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0"/>
+      <c r="B26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H26" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K26" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0"/>
+      <c r="B27" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K27" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0"/>
+      <c r="B28" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H28" s="9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" s="9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0"/>
+      <c r="B29" s="0"/>
+      <c r="C29" s="0"/>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
+      <c r="C30" s="0"/>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
+      <c r="I32" s="0"/>
+      <c r="J32" s="0"/>
+      <c r="K32" s="0"/>
+    </row>
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0"/>
+      <c r="B33" s="0"/>
+      <c r="C33" s="0"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
+      <c r="I33" s="0"/>
+      <c r="J33" s="0"/>
+      <c r="K33" s="0"/>
+    </row>
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+      <c r="F34" s="0"/>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
+      <c r="I34" s="0"/>
+      <c r="J34" s="0"/>
+      <c r="K34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+      <c r="F35" s="0"/>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
+      <c r="I35" s="0"/>
+      <c r="J35" s="0"/>
+      <c r="K35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+      <c r="F36" s="0"/>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
+      <c r="I36" s="0"/>
+      <c r="J36" s="0"/>
+      <c r="K36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+      <c r="F37" s="0"/>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
+      <c r="I37" s="0"/>
+      <c r="J37" s="0"/>
+      <c r="K37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+      <c r="F38" s="0"/>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
+      <c r="I38" s="0"/>
+      <c r="J38" s="0"/>
+      <c r="K38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+      <c r="F39" s="0"/>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
+      <c r="I39" s="0"/>
+      <c r="J39" s="0"/>
+      <c r="K39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+      <c r="F40" s="0"/>
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
+      <c r="I40" s="0"/>
+      <c r="J40" s="0"/>
+      <c r="K40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+      <c r="F41" s="0"/>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
+      <c r="I41" s="0"/>
+      <c r="J41" s="0"/>
+      <c r="K41" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1097,10 +2060,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1115,10 +2078,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1129,7 +2092,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1137,10 +2100,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1148,10 +2111,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1159,10 +2122,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1170,10 +2133,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1181,10 +2144,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1192,10 +2155,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1203,10 +2166,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,10 +2177,208 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>65</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1238,8 +2399,8 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1253,7 +2414,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1261,7 +2422,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1277,7 +2438,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>68</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1285,7 +2446,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1304,10 +2465,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1322,10 +2483,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1336,7 +2497,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1344,10 +2505,10 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1355,10 +2516,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1366,10 +2527,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1377,10 +2538,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1388,10 +2549,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1399,10 +2560,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1410,10 +2571,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1421,10 +2582,208 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1443,10 +2802,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1462,13 +2821,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>66</v>
+        <v>129</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>71</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1479,10 +2838,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1490,13 +2849,13 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1504,13 +2863,13 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1518,13 +2877,13 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1532,13 +2891,13 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1546,13 +2905,13 @@
         <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1560,13 +2919,13 @@
         <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,13 +2933,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1588,13 +2947,265 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>72</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finishing document and its each own sub unit page for creating but theres still some optimnization needed in mapcombos for units
</commit_message>
<xml_diff>
--- a/database/masters/base-seeder.xlsx
+++ b/database/masters/base-seeder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="module" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="140">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -172,6 +172,18 @@
   </si>
   <si>
     <t xml:space="preserve">unit/:unit/asset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit Documents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">infrastructure-unit-document</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unit/:unit/document</t>
   </si>
   <si>
     <t xml:space="preserve">Unit Asset Documents</t>
@@ -778,7 +790,7 @@
   </sheetPr>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -887,7 +899,7 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -962,10 +974,12 @@
       <c r="G2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="9" t="b">
+      <c r="H2" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="I2" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="K2" s="10" t="b">
@@ -995,10 +1009,12 @@
       <c r="G3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9" t="b">
+      <c r="H3" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="9" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K3" s="10" t="b">
@@ -1028,10 +1044,12 @@
       <c r="G4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9" t="b">
+      <c r="H4" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="9" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K4" s="10" t="b">
@@ -1061,10 +1079,12 @@
       <c r="G5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I5" s="9" t="b">
+      <c r="H5" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="9" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K5" s="10" t="b">
@@ -1094,10 +1114,12 @@
       <c r="G6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H6" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9" t="b">
+      <c r="H6" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="K6" s="10" t="b">
@@ -1127,11 +1149,13 @@
       <c r="G7" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I7" s="9" t="b">
-        <v>0</v>
+      <c r="H7" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="9" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="K7" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1160,10 +1184,12 @@
       <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="9" t="b">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9" t="b">
+      <c r="H8" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -1182,10 +1208,10 @@
         <v>49</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>33</v>
@@ -1194,16 +1220,18 @@
         <v>12</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I9" s="9" t="b">
+        <v>52</v>
+      </c>
+      <c r="H9" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="K9" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1215,13 +1243,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>33</v>
@@ -1230,16 +1258,18 @@
         <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I10" s="9" t="b">
+        <v>55</v>
+      </c>
+      <c r="H10" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="K10" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1251,7 +1281,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>56</v>
@@ -1268,10 +1298,12 @@
       <c r="G11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H11" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" s="9" t="b">
+      <c r="H11" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J11" s="1" t="s">
@@ -1304,14 +1336,16 @@
       <c r="G12" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="H12" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I12" s="9" t="b">
+      <c r="H12" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="K12" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1340,14 +1374,16 @@
       <c r="G13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I13" s="9" t="b">
+      <c r="H13" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K13" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1376,14 +1412,16 @@
       <c r="G14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I14" s="9" t="b">
+      <c r="H14" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="K14" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1412,14 +1450,16 @@
       <c r="G15" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="H15" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I15" s="9" t="b">
+      <c r="H15" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="K15" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1448,14 +1488,16 @@
       <c r="G16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="H16" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="9" t="b">
+      <c r="H16" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="K16" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1470,10 +1512,10 @@
         <v>79</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>33</v>
@@ -1482,16 +1524,18 @@
         <v>12</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H17" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="9" t="b">
+        <v>82</v>
+      </c>
+      <c r="H17" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K17" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1503,10 +1547,10 @@
         <v>12</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>84</v>
@@ -1520,14 +1564,16 @@
       <c r="G18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="H18" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="9" t="b">
+      <c r="H18" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="K18" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1535,7 +1581,9 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0"/>
+      <c r="A19" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>86</v>
       </c>
@@ -1554,14 +1602,16 @@
       <c r="G19" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="9" t="b">
+      <c r="H19" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="K19" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1569,7 +1619,9 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0"/>
+      <c r="A20" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>90</v>
       </c>
@@ -1588,14 +1640,16 @@
       <c r="G20" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="H20" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="9" t="b">
+      <c r="H20" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="K20" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1604,7 +1658,9 @@
       <c r="L20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0"/>
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>94</v>
       </c>
@@ -1621,16 +1677,18 @@
         <v>12</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="9" t="b">
+        <v>97</v>
+      </c>
+      <c r="H21" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="K21" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1638,15 +1696,17 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0"/>
+      <c r="A22" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B22" s="1" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>33</v>
@@ -1655,16 +1715,18 @@
         <v>12</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H22" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="9" t="b">
+        <v>82</v>
+      </c>
+      <c r="H22" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="K22" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1672,7 +1734,9 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0"/>
+      <c r="A23" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>101</v>
       </c>
@@ -1691,14 +1755,16 @@
       <c r="G23" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="H23" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="9" t="b">
+      <c r="H23" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="K23" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1706,7 +1772,9 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0"/>
+      <c r="A24" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>105</v>
       </c>
@@ -1725,14 +1793,16 @@
       <c r="G24" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H24" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="9" t="b">
+      <c r="H24" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>41</v>
+        <v>77</v>
       </c>
       <c r="K24" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1740,7 +1810,9 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0"/>
+      <c r="A25" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>109</v>
       </c>
@@ -1759,14 +1831,16 @@
       <c r="G25" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="9" t="b">
+      <c r="H25" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="K25" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1774,7 +1848,9 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0"/>
+      <c r="A26" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>113</v>
       </c>
@@ -1791,16 +1867,18 @@
         <v>12</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H26" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="9" t="b">
+        <v>116</v>
+      </c>
+      <c r="H26" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="K26" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1808,15 +1886,17 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0"/>
+      <c r="A27" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B27" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>33</v>
@@ -1825,12 +1905,14 @@
         <v>12</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H27" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="9" t="b">
+        <v>66</v>
+      </c>
+      <c r="H27" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J27" s="1" t="s">
@@ -1842,7 +1924,9 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0"/>
+      <c r="A28" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B28" s="1" t="s">
         <v>120</v>
       </c>
@@ -1861,14 +1945,16 @@
       <c r="G28" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="H28" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" s="9" t="b">
+      <c r="H28" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="9" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="K28" s="10" t="b">
         <f aca="false">TRUE()</f>
@@ -1876,173 +1962,90 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0"/>
-      <c r="B29" s="0"/>
-      <c r="C29" s="0"/>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
-      <c r="I29" s="0"/>
-      <c r="J29" s="0"/>
-      <c r="K29" s="0"/>
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H29" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="9" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="K29" s="10" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
-      <c r="C30" s="0"/>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-      <c r="G30" s="0"/>
-      <c r="H30" s="0"/>
-      <c r="I30" s="0"/>
-      <c r="J30" s="0"/>
-      <c r="K30" s="0"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
-      <c r="H31" s="0"/>
-      <c r="I31" s="0"/>
-      <c r="J31" s="0"/>
-      <c r="K31" s="0"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0"/>
-      <c r="B32" s="0"/>
-      <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
-      <c r="E32" s="0"/>
-      <c r="F32" s="0"/>
-      <c r="G32" s="0"/>
-      <c r="H32" s="0"/>
-      <c r="I32" s="0"/>
-      <c r="J32" s="0"/>
-      <c r="K32" s="0"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0"/>
-      <c r="B33" s="0"/>
-      <c r="C33" s="0"/>
-      <c r="D33" s="0"/>
-      <c r="E33" s="0"/>
-      <c r="F33" s="0"/>
-      <c r="G33" s="0"/>
-      <c r="H33" s="0"/>
-      <c r="I33" s="0"/>
-      <c r="J33" s="0"/>
-      <c r="K33" s="0"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0"/>
-      <c r="B34" s="0"/>
-      <c r="C34" s="0"/>
-      <c r="D34" s="0"/>
-      <c r="E34" s="0"/>
-      <c r="F34" s="0"/>
-      <c r="G34" s="0"/>
-      <c r="H34" s="0"/>
-      <c r="I34" s="0"/>
-      <c r="J34" s="0"/>
-      <c r="K34" s="0"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0"/>
-      <c r="B35" s="0"/>
-      <c r="C35" s="0"/>
-      <c r="D35" s="0"/>
-      <c r="E35" s="0"/>
-      <c r="F35" s="0"/>
-      <c r="G35" s="0"/>
-      <c r="H35" s="0"/>
-      <c r="I35" s="0"/>
-      <c r="J35" s="0"/>
-      <c r="K35" s="0"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0"/>
-      <c r="B36" s="0"/>
-      <c r="C36" s="0"/>
-      <c r="D36" s="0"/>
-      <c r="E36" s="0"/>
-      <c r="F36" s="0"/>
-      <c r="G36" s="0"/>
-      <c r="H36" s="0"/>
-      <c r="I36" s="0"/>
-      <c r="J36" s="0"/>
-      <c r="K36" s="0"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
-      <c r="D37" s="0"/>
-      <c r="E37" s="0"/>
-      <c r="F37" s="0"/>
-      <c r="G37" s="0"/>
-      <c r="H37" s="0"/>
-      <c r="I37" s="0"/>
-      <c r="J37" s="0"/>
-      <c r="K37" s="0"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0"/>
-      <c r="B38" s="0"/>
-      <c r="C38" s="0"/>
-      <c r="D38" s="0"/>
-      <c r="E38" s="0"/>
-      <c r="F38" s="0"/>
-      <c r="G38" s="0"/>
-      <c r="H38" s="0"/>
-      <c r="I38" s="0"/>
-      <c r="J38" s="0"/>
-      <c r="K38" s="0"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0"/>
-      <c r="B39" s="0"/>
-      <c r="C39" s="0"/>
-      <c r="D39" s="0"/>
-      <c r="E39" s="0"/>
-      <c r="F39" s="0"/>
-      <c r="G39" s="0"/>
-      <c r="H39" s="0"/>
-      <c r="I39" s="0"/>
-      <c r="J39" s="0"/>
-      <c r="K39" s="0"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0"/>
-      <c r="B40" s="0"/>
-      <c r="C40" s="0"/>
-      <c r="D40" s="0"/>
-      <c r="E40" s="0"/>
-      <c r="F40" s="0"/>
-      <c r="G40" s="0"/>
-      <c r="H40" s="0"/>
-      <c r="I40" s="0"/>
-      <c r="J40" s="0"/>
-      <c r="K40" s="0"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0"/>
-      <c r="B41" s="0"/>
-      <c r="C41" s="0"/>
-      <c r="D41" s="0"/>
-      <c r="E41" s="0"/>
-      <c r="F41" s="0"/>
-      <c r="G41" s="0"/>
-      <c r="H41" s="0"/>
-      <c r="I41" s="0"/>
-      <c r="J41" s="0"/>
-      <c r="K41" s="0"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2060,10 +2063,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2078,10 +2081,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2092,7 +2095,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2103,7 +2106,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2114,7 +2117,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2125,7 +2128,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2136,7 +2139,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2147,7 +2150,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2158,7 +2161,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2166,10 +2169,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2177,10 +2180,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,7 +2194,7 @@
         <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2202,7 +2205,7 @@
         <v>61</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2213,7 +2216,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2224,7 +2227,7 @@
         <v>69</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2235,7 +2238,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2246,7 +2249,7 @@
         <v>77</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2254,10 +2257,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2268,7 +2271,7 @@
         <v>84</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2279,7 +2282,7 @@
         <v>88</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2290,7 +2293,7 @@
         <v>92</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2301,7 +2304,7 @@
         <v>96</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,10 +2312,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2323,7 +2326,7 @@
         <v>103</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,7 +2337,7 @@
         <v>107</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,7 +2348,7 @@
         <v>111</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2356,7 +2359,7 @@
         <v>115</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2364,10 +2367,10 @@
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2378,7 +2381,18 @@
         <v>122</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>128</v>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -2399,7 +2413,7 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -2414,7 +2428,7 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2422,7 +2436,7 @@
         <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2438,7 +2452,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,7 +2460,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2465,10 +2479,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2483,10 +2497,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2497,7 +2511,7 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2508,7 +2522,7 @@
         <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2519,7 +2533,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2530,7 +2544,7 @@
         <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2541,7 +2555,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2552,7 +2566,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2563,7 +2577,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2571,10 +2585,10 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2582,10 +2596,10 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2596,7 +2610,7 @@
         <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2607,7 +2621,7 @@
         <v>61</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,7 +2632,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2629,7 +2643,7 @@
         <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,7 +2654,7 @@
         <v>73</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2651,7 +2665,7 @@
         <v>77</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2659,10 +2673,10 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2673,7 +2687,7 @@
         <v>84</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2684,7 +2698,7 @@
         <v>88</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,7 +2709,7 @@
         <v>92</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2706,7 +2720,7 @@
         <v>96</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2714,10 +2728,10 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2728,7 +2742,7 @@
         <v>103</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2739,7 +2753,7 @@
         <v>107</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2750,7 +2764,7 @@
         <v>111</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2761,7 +2775,7 @@
         <v>115</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2769,10 +2783,10 @@
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2783,7 +2797,18 @@
         <v>122</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2802,10 +2827,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D28"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A19" activeCellId="0" sqref="A19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J38" activeCellId="0" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2821,13 +2846,13 @@
         <v>18</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2838,10 +2863,10 @@
         <v>25</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2852,10 +2877,10 @@
         <v>28</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2866,10 +2891,10 @@
         <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2880,10 +2905,10 @@
         <v>37</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2894,10 +2919,10 @@
         <v>41</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2908,10 +2933,10 @@
         <v>44</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2922,10 +2947,10 @@
         <v>47</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2933,13 +2958,13 @@
         <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2947,13 +2972,13 @@
         <v>12</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2964,10 +2989,10 @@
         <v>57</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2978,10 +3003,10 @@
         <v>61</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2992,10 +3017,10 @@
         <v>65</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,10 +3031,10 @@
         <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3020,10 +3045,10 @@
         <v>73</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3034,10 +3059,10 @@
         <v>77</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3045,13 +3070,13 @@
         <v>12</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3062,10 +3087,10 @@
         <v>84</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3076,10 +3101,10 @@
         <v>88</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3090,10 +3115,10 @@
         <v>92</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3104,10 +3129,10 @@
         <v>96</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3115,13 +3140,13 @@
         <v>12</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3132,10 +3157,10 @@
         <v>103</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3146,10 +3171,10 @@
         <v>107</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3160,10 +3185,10 @@
         <v>111</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3174,10 +3199,10 @@
         <v>115</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3185,13 +3210,13 @@
         <v>12</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3202,10 +3227,24 @@
         <v>122</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sub routing in api php router
</commit_message>
<xml_diff>
--- a/database/masters/base-seeder.xlsx
+++ b/database/masters/base-seeder.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="module" sheetId="1" state="visible" r:id="rId3"/>
@@ -465,7 +465,7 @@
     <t xml:space="preserve">infrastructure-unit-asset-tax-note</t>
   </si>
   <si>
-    <t xml:space="preserve">unit/:unit/asset/:asset/tax/:note/note</t>
+    <t xml:space="preserve">unit/:unit/asset/:asset/tax/:record/note</t>
   </si>
   <si>
     <t xml:space="preserve">Unit Asset Tax Record Used</t>
@@ -1105,7 +1105,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="1" sqref="D53:D54 C23"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1213,8 +1213,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="1" sqref="D53:D54 D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G34" activeCellId="0" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3467,7 +3467,7 @@
   <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D53:D54 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4090,7 +4090,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I22" activeCellId="1" sqref="D53:D54 I22"/>
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4163,7 +4163,7 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="D53:D54 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4829,8 +4829,8 @@
   </sheetPr>
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53:D54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D53" activeCellId="0" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>